<commit_message>
worked on stock import
</commit_message>
<xml_diff>
--- a/OraRegaAV/FormatFiles/PartDetailsFormatFile.xlsx
+++ b/OraRegaAV/FormatFiles/PartDetailsFormatFile.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>PartNumber</t>
   </si>
@@ -51,9 +51,6 @@
     <t>DocketNo</t>
   </si>
   <si>
-    <t>StockPartStatus</t>
-  </si>
-  <si>
     <t>PurchasePrice</t>
   </si>
   <si>
@@ -87,16 +84,16 @@
     <t>Quikserv</t>
   </si>
   <si>
-    <t>Sakinaka</t>
-  </si>
-  <si>
     <t>avxxx</t>
   </si>
   <si>
     <t>D1014</t>
   </si>
   <si>
-    <t>DOA</t>
+    <t>Goa</t>
+  </si>
+  <si>
+    <t>14/05/2024</t>
   </si>
 </sst>
 </file>
@@ -134,7 +131,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -452,15 +449,14 @@
     <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -488,7 +484,7 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="K1" t="s">
@@ -506,70 +502,65 @@
       <c r="O1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>19</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>20</v>
-      </c>
-      <c r="E2" t="s">
-        <v>21</v>
       </c>
       <c r="F2">
         <v>100</v>
       </c>
       <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
         <v>22</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" t="s">
         <v>23</v>
       </c>
-      <c r="I2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" s="1">
-        <v>45364</v>
-      </c>
-      <c r="K2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" t="s">
-        <v>26</v>
+      <c r="L2">
+        <v>50</v>
       </c>
       <c r="M2">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="N2">
-        <v>1</v>
-      </c>
-      <c r="O2">
         <v>323454</v>
       </c>
-      <c r="P2" t="s">
-        <v>16</v>
+      <c r="O2" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P1:P1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O1:O1048576">
       <formula1>"Active,In Active"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L1:L1048576">
-      <formula1>"Good,DOA,Defective"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576">
+      <formula1>"Good"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added GSTType new field in quotation
</commit_message>
<xml_diff>
--- a/OraRegaAV/FormatFiles/PartDetailsFormatFile.xlsx
+++ b/OraRegaAV/FormatFiles/PartDetailsFormatFile.xlsx
@@ -93,7 +93,7 @@
     <t>Goa</t>
   </si>
   <si>
-    <t>14/05/2024</t>
+    <t>2024-05-30</t>
   </si>
 </sst>
 </file>
@@ -436,7 +436,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>